<commit_message>
add materials for session 02
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fedietri/GitHub/24-1-nmok/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F2E433-811E-5640-9D7E-A2290426B07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C599B8F0-263C-9A41-A979-58461ED91B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>exercises/e01.html</t>
   </si>
@@ -123,6 +123,15 @@
   </si>
   <si>
     <t>exercises/e07.html</t>
+  </si>
+  <si>
+    <t>slides/slides.html#/sitzung-02-warum-wir-mediennutzung-unterhaltsam-finden</t>
+  </si>
+  <si>
+    <t>exercises/e02.html</t>
+  </si>
+  <si>
+    <t>prep/p03.html</t>
   </si>
 </sst>
 </file>
@@ -478,7 +487,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -539,6 +548,12 @@
       <c r="D3" t="s">
         <v>1</v>
       </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
       <c r="G3" t="s">
         <v>13</v>
       </c>
@@ -552,6 +567,9 @@
       </c>
       <c r="C4" t="s">
         <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
       </c>
       <c r="G4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
add materials for session 03
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fedietri/GitHub/24-1-nmok/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C599B8F0-263C-9A41-A979-58461ED91B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325018B1-13ED-D549-9AAC-756EBD71A8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>exercises/e01.html</t>
   </si>
@@ -132,6 +132,15 @@
   </si>
   <si>
     <t>prep/p03.html</t>
+  </si>
+  <si>
+    <t>prep/p04.html</t>
+  </si>
+  <si>
+    <t>exercises/e03.html</t>
+  </si>
+  <si>
+    <t>slides/slides.html#/sitzung-03-warum-wir-unterschiedliche-inhalte-in-manchen-situationen-unterhaltsam-finden</t>
   </si>
 </sst>
 </file>
@@ -487,7 +496,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,6 +580,12 @@
       <c r="D4" t="s">
         <v>31</v>
       </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
       <c r="G4" t="s">
         <v>13</v>
       </c>
@@ -595,6 +610,9 @@
       </c>
       <c r="C6" t="s">
         <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
       </c>
       <c r="G6" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
add materials for session 04
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fedietri/GitHub/24-1-nmok/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325018B1-13ED-D549-9AAC-756EBD71A8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7207C0-F75F-AC4C-BB99-F83BCC11712A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>exercises/e01.html</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>slides/slides.html#/sitzung-03-warum-wir-unterschiedliche-inhalte-in-manchen-situationen-unterhaltsam-finden</t>
+  </si>
+  <si>
+    <t>prep/p05.html</t>
+  </si>
+  <si>
+    <t>exercises/e04.html</t>
+  </si>
+  <si>
+    <t>slides/slides.html#/sitzung-05-warum-wir-nicht-alle-medienerlebnisse-als-unterhaltung-bezeichnen-sollten</t>
   </si>
 </sst>
 </file>
@@ -496,7 +505,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -614,6 +623,12 @@
       <c r="D6" t="s">
         <v>32</v>
       </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
       <c r="G6" t="s">
         <v>13</v>
       </c>
@@ -627,6 +642,9 @@
       </c>
       <c r="C7" t="s">
         <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
       </c>
       <c r="G7" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
add materials for session 06
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fedietri/GitHub/24-1-nmok/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7207C0-F75F-AC4C-BB99-F83BCC11712A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA078F6-B612-4E4D-A6A1-0643E2015F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>exercises/e01.html</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>slides/slides.html#/sitzung-05-warum-wir-nicht-alle-medienerlebnisse-als-unterhaltung-bezeichnen-sollten</t>
+  </si>
+  <si>
+    <t>prep/p08.html</t>
+  </si>
+  <si>
+    <t>slides/slides.html#/sitzung-06-warum-diese-medienerlebnisse-manchmal-trotzdem-unterhaltsam-sein-können</t>
   </si>
 </sst>
 </file>
@@ -505,7 +511,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -646,6 +652,9 @@
       <c r="D7" t="s">
         <v>35</v>
       </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
       <c r="G7" t="s">
         <v>13</v>
       </c>
@@ -673,6 +682,9 @@
       </c>
       <c r="C9" t="s">
         <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
       </c>
       <c r="G9" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
add materials for session 08
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fedietri/GitHub/24-1-nmok/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA078F6-B612-4E4D-A6A1-0643E2015F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A20744-7571-AB40-8350-2213333DCCAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>exercises/e01.html</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>slides/slides.html#/sitzung-06-warum-diese-medienerlebnisse-manchmal-trotzdem-unterhaltsam-sein-können</t>
+  </si>
+  <si>
+    <t>prep/p09.html</t>
+  </si>
+  <si>
+    <t>slides/slides.html#/sitzung-08-warum-medienunterhaltung-in-algorithmisch-kuratierten-umgebungen-anders-ist</t>
   </si>
 </sst>
 </file>
@@ -511,7 +517,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -686,6 +692,9 @@
       <c r="D9" t="s">
         <v>38</v>
       </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
       <c r="G9" t="s">
         <v>19</v>
       </c>
@@ -699,6 +708,9 @@
       </c>
       <c r="C10" t="s">
         <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
       </c>
       <c r="G10" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
add submission for session 08
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fedietri/GitHub/24-1-nmok/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A20744-7571-AB40-8350-2213333DCCAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2047B4F-AF0D-CE46-B9D2-B77DE188C719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="17500" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>exercises/e01.html</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>slides/slides.html#/sitzung-08-warum-medienunterhaltung-in-algorithmisch-kuratierten-umgebungen-anders-ist</t>
+  </si>
+  <si>
+    <t>exercises/e08.html</t>
   </si>
 </sst>
 </file>
@@ -517,7 +520,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -695,6 +698,9 @@
       <c r="E9" t="s">
         <v>41</v>
       </c>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
       <c r="G9" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
add materials for session 11
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fedietri/GitHub/24-1-nmok/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36113956-A85E-B849-B572-403DC5DD90D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE9F3A0-938C-7C45-A55D-B11DC554B248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="17500" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t>exercises/e01.html</t>
   </si>
@@ -183,6 +183,15 @@
   </si>
   <si>
     <t>slides/slides.html#/sitzung-10-human-agency-wie-menschen-sich-auf-algorithmisch-kuratierten-plattformen-unterhalten</t>
+  </si>
+  <si>
+    <t>exercises/e11.html</t>
+  </si>
+  <si>
+    <t>prep/p12.html</t>
+  </si>
+  <si>
+    <t>slides/slides.html#/sitzung-11-machine-agency-wie-algorithmen-das-unterhaltungserleben-beeiflussen-können</t>
   </si>
 </sst>
 </file>
@@ -538,7 +547,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -782,6 +791,12 @@
       <c r="D12" t="s">
         <v>46</v>
       </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
+        <v>49</v>
+      </c>
       <c r="G12" t="s">
         <v>19</v>
       </c>
@@ -795,6 +810,9 @@
       </c>
       <c r="C13" t="s">
         <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
       </c>
       <c r="G13" t="s">
         <v>19</v>

</xml_diff>